<commit_message>
InventoriesForm-Continued coding adding inventory items
</commit_message>
<xml_diff>
--- a/Stock Location labels.xlsx
+++ b/Stock Location labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\System Developments\VEHICLE MANAGEMENT SYSTEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69ACA43A-32D2-4DC5-AA80-3349057E023F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6368A82D-0ADD-4CCA-8FAF-3924F3C12467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{B4C8AD9B-629E-4540-BB55-ECB34A71DB83}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Box-1</t>
   </si>
@@ -68,18 +68,6 @@
   </si>
   <si>
     <t>Box-12</t>
-  </si>
-  <si>
-    <t>Rack-Rk</t>
-  </si>
-  <si>
-    <t>Steel Cabinet-Sc</t>
-  </si>
-  <si>
-    <t>Tool Box-Tb</t>
-  </si>
-  <si>
-    <t>Ceiling</t>
   </si>
 </sst>
 </file>
@@ -459,97 +447,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5475EC22-F5CD-40D3-920A-9A1B65875934}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="8" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" ht="44.25" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>